<commit_message>
Fixed Maintenance Activity data dictionary
</commit_message>
<xml_diff>
--- a/Data Dictionary Maintenance Activity.xlsx
+++ b/Data Dictionary Maintenance Activity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\the-b\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\the-b\Desktop\SE\github\SE_Gruppo10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B4EA16-EE40-41BC-A734-84533024155C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E2C813-FDF8-4D24-88A9-D763E5FBE59A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11600" yWindow="3040" windowWidth="14400" windowHeight="7360" xr2:uid="{99D2DFC3-8DA2-4FEB-983D-B3E8222FFD5E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{99D2DFC3-8DA2-4FEB-983D-B3E8222FFD5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>Data Dictionary Maintenance Activity</t>
   </si>
@@ -126,18 +126,9 @@
     <t>Interruptible</t>
   </si>
   <si>
-    <t>yes/no</t>
-  </si>
-  <si>
     <t>planned</t>
   </si>
   <si>
-    <t>Is the Activity interruptible by a Emergency Work Order?</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>Materials</t>
   </si>
   <si>
@@ -172,6 +163,51 @@
   </si>
   <si>
     <t>Planned electrical Maintenance Activity at Management's area</t>
+  </si>
+  <si>
+    <t>Week Day</t>
+  </si>
+  <si>
+    <t>Bool</t>
+  </si>
+  <si>
+    <t>True/False</t>
+  </si>
+  <si>
+    <t>Is the Activity interruptible by a Emergency Work Order? True -&gt; Yes ; False -&gt; No</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>monday/tuesday/wednesday/thursday/friday/saturday/sunday</t>
+  </si>
+  <si>
+    <t>Week day in which the activity will be performed</t>
+  </si>
+  <si>
+    <t>tuesday</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>8/9/10…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start time, in hour, of the activity </t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Maintainer Username</t>
+  </si>
+  <si>
+    <t>Username of the maintainer that will perform the activity</t>
+  </si>
+  <si>
+    <t>mario123</t>
   </si>
 </sst>
 </file>
@@ -291,23 +327,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C05BB4-1D3B-43F3-B954-E5D7905DC471}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,7 +670,7 @@
     <col min="1" max="1" width="12.7265625" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" customWidth="1"/>
-    <col min="4" max="4" width="38.7265625" customWidth="1"/>
+    <col min="4" max="4" width="34.36328125" customWidth="1"/>
     <col min="6" max="6" width="12.54296875" customWidth="1"/>
     <col min="7" max="7" width="50" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
@@ -673,232 +709,298 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="7"/>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="7"/>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="7"/>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="7"/>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="7"/>
+      <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4" t="s">
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="5">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
+    </row>
+    <row r="13" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="8"/>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>44</v>
+      <c r="G16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="A4:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed Data Dictionary for maintenance activity
</commit_message>
<xml_diff>
--- a/Data Dictionary Maintenance Activity.xlsx
+++ b/Data Dictionary Maintenance Activity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\the-b\Desktop\SE\github\SE_Gruppo10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E2C813-FDF8-4D24-88A9-D763E5FBE59A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F82081-AD8F-4AA8-B6DF-B0BD09C2F04A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{99D2DFC3-8DA2-4FEB-983D-B3E8222FFD5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{99D2DFC3-8DA2-4FEB-983D-B3E8222FFD5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
-  <si>
-    <t>Data Dictionary Maintenance Activity</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
   <si>
     <t>Table Name</t>
   </si>
@@ -75,12 +72,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Maintenance Activity</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Int</t>
   </si>
   <si>
@@ -90,24 +81,15 @@
     <t>Unique Identifier for Maintenance Activities</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>planned/unplanned/extra</t>
   </si>
   <si>
-    <t>Site</t>
-  </si>
-  <si>
     <t>Factory's site and area in which the Activity will be performed</t>
   </si>
   <si>
     <t>Management</t>
   </si>
   <si>
-    <t>Typology</t>
-  </si>
-  <si>
     <t>Type of the Maintenance Activity</t>
   </si>
   <si>
@@ -117,36 +99,21 @@
     <t>Description of the Activity</t>
   </si>
   <si>
-    <t>Estimated Time</t>
-  </si>
-  <si>
     <t>Expected Activity's lifetime in minutes</t>
   </si>
   <si>
-    <t>Interruptible</t>
-  </si>
-  <si>
     <t>planned</t>
   </si>
   <si>
-    <t>Materials</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>List of materials to be used during the Activity</t>
   </si>
   <si>
-    <t>Week</t>
-  </si>
-  <si>
     <t>Week (1 to 52) in which the activity will be performed</t>
   </si>
   <si>
-    <t>Workspace Notes</t>
-  </si>
-  <si>
     <t>spikes, drill</t>
   </si>
   <si>
@@ -159,15 +126,9 @@
     <t>electrical</t>
   </si>
   <si>
-    <t>Site: Management Typology: electrical Expected Time: 30</t>
-  </si>
-  <si>
     <t>Planned electrical Maintenance Activity at Management's area</t>
   </si>
   <si>
-    <t>Week Day</t>
-  </si>
-  <si>
     <t>Bool</t>
   </si>
   <si>
@@ -189,25 +150,67 @@
     <t>tuesday</t>
   </si>
   <si>
-    <t>Start Time</t>
-  </si>
-  <si>
     <t>8/9/10…</t>
   </si>
   <si>
     <t xml:space="preserve">Start time, in hour, of the activity </t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Maintainer Username</t>
-  </si>
-  <si>
     <t>Username of the maintainer that will perform the activity</t>
   </si>
   <si>
     <t>mario123</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>activity_id</t>
+  </si>
+  <si>
+    <t>maintenance_activity</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>typology</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>estimated_time</t>
+  </si>
+  <si>
+    <t>interruptible</t>
+  </si>
+  <si>
+    <t>materials</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>week_day</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>maintainer_username</t>
+  </si>
+  <si>
+    <t>workspace_notes</t>
+  </si>
+  <si>
+    <t>These are notes for the activity</t>
+  </si>
+  <si>
+    <t>Data Dictionary For Maintenance Activity</t>
   </si>
 </sst>
 </file>
@@ -319,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -345,9 +348,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -363,7 +372,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -661,346 +670,356 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C05BB4-1D3B-43F3-B954-E5D7905DC471}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" customWidth="1"/>
-    <col min="4" max="4" width="34.36328125" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="50" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="H4" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="5">
+        <v>21</v>
+      </c>
+      <c r="H9" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="5">
+        <v>25</v>
+      </c>
+      <c r="H12" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+      <c r="H15" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="F16" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:A16"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed table name in maintenance activity data dictionary
</commit_message>
<xml_diff>
--- a/Data Dictionary Maintenance Activity.xlsx
+++ b/Data Dictionary Maintenance Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F82081-AD8F-4AA8-B6DF-B0BD09C2F04A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3E8BCE-0F99-46AA-B295-05E678513F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{99D2DFC3-8DA2-4FEB-983D-B3E8222FFD5E}"/>
+    <workbookView xWindow="5790" yWindow="2775" windowWidth="28800" windowHeight="15435" xr2:uid="{99D2DFC3-8DA2-4FEB-983D-B3E8222FFD5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -168,9 +168,6 @@
     <t>activity_id</t>
   </si>
   <si>
-    <t>maintenance_activity</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>Data Dictionary For Maintenance Activity</t>
+  </si>
+  <si>
+    <t>maintenance_activities</t>
   </si>
 </sst>
 </file>
@@ -339,6 +339,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -347,9 +350,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,7 +671,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -725,8 +725,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>44</v>
+      <c r="A4" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>43</v>
@@ -746,14 +746,14 @@
       <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
@@ -773,9 +773,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -795,9 +795,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
@@ -817,9 +817,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>8</v>
@@ -839,9 +839,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>12</v>
@@ -856,14 +856,14 @@
       <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="6">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>31</v>
@@ -883,9 +883,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -905,9 +905,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
@@ -922,14 +922,14 @@
       <c r="G12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="6">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>8</v>
@@ -945,13 +945,13 @@
         <v>27</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>8</v>
@@ -971,9 +971,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>12</v>
@@ -988,14 +988,14 @@
       <c r="G15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="6">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>

</xml_diff>